<commit_message>
Knesset 1 bug fix
</commit_message>
<xml_diff>
--- a/Processed Data/Knessets.xlsx
+++ b/Processed Data/Knessets.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24124"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\Year A Sem B\Intro to Statistics\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABAYT\Desktop\projectstat\Statistics-Project\Processed Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7EFC774F-C420-4145-9DDC-A61750172EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84D96B57-655F-496B-A803-0DE0088862BF}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{7D0C82D7-6527-4A3C-A2F5-D87BBBA0860B}"/>
+    <workbookView xWindow="5760" yWindow="3390" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$288</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="147">
   <si>
     <t>Knesset</t>
   </si>
@@ -483,12 +482,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -496,14 +495,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -565,8 +564,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ניטראלי" xfId="1" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -877,28 +876,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177842A7-6D16-49EA-B1EA-3B800BE62D51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="11.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -958,9 +957,11 @@
       <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -988,7 +989,7 @@
       </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1016,9 +1017,11 @@
       <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="J4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1046,7 +1049,7 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -1074,7 +1077,7 @@
       </c>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1100,9 +1103,11 @@
         <v>22</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -1132,7 +1137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -1160,7 +1165,7 @@
       </c>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1184,9 +1189,11 @@
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -1212,7 +1219,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -1236,9 +1243,11 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="J12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -1266,7 +1275,7 @@
       </c>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>2</v>
       </c>
@@ -1298,7 +1307,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -1326,7 +1335,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>2</v>
       </c>
@@ -1358,7 +1367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -1388,7 +1397,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>2</v>
       </c>
@@ -1416,7 +1425,7 @@
       </c>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>2</v>
       </c>
@@ -1446,7 +1455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -1478,7 +1487,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -1510,7 +1519,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2</v>
       </c>
@@ -1538,7 +1547,7 @@
       </c>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -1568,7 +1577,7 @@
       </c>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -1596,7 +1605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -1624,7 +1633,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>2</v>
       </c>
@@ -1682,7 +1691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -1714,7 +1723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>3</v>
       </c>
@@ -1740,7 +1749,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>3</v>
       </c>
@@ -1770,7 +1779,7 @@
       </c>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>3</v>
       </c>
@@ -1798,7 +1807,7 @@
       </c>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>3</v>
       </c>
@@ -1828,7 +1837,7 @@
       </c>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>3</v>
       </c>
@@ -1858,7 +1867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>3</v>
       </c>
@@ -1890,7 +1899,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>3</v>
       </c>
@@ -1922,7 +1931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>3</v>
       </c>
@@ -1950,7 +1959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>3</v>
       </c>
@@ -1980,7 +1989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>3</v>
       </c>
@@ -2008,7 +2017,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>3</v>
       </c>
@@ -2034,7 +2043,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>3</v>
       </c>
@@ -2064,7 +2073,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>4</v>
       </c>
@@ -2090,7 +2099,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>4</v>
       </c>
@@ -2122,7 +2131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>4</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>4</v>
       </c>
@@ -2184,7 +2193,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>4</v>
       </c>
@@ -2214,7 +2223,7 @@
       </c>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>4</v>
       </c>
@@ -2244,7 +2253,7 @@
       </c>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>4</v>
       </c>
@@ -2272,7 +2281,7 @@
       </c>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>4</v>
       </c>
@@ -2298,7 +2307,7 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>4</v>
       </c>
@@ -2324,7 +2333,7 @@
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>4</v>
       </c>
@@ -2352,7 +2361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>4</v>
       </c>
@@ -2382,7 +2391,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>4</v>
       </c>
@@ -2412,7 +2421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>5</v>
       </c>
@@ -2444,7 +2453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>5</v>
       </c>
@@ -2474,7 +2483,7 @@
       </c>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>5</v>
       </c>
@@ -2504,7 +2513,7 @@
       </c>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>5</v>
       </c>
@@ -2532,7 +2541,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>5</v>
       </c>
@@ -2558,7 +2567,7 @@
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>5</v>
       </c>
@@ -2586,7 +2595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>5</v>
       </c>
@@ -2614,7 +2623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>5</v>
       </c>
@@ -2642,7 +2651,7 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>5</v>
       </c>
@@ -2668,7 +2677,7 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>5</v>
       </c>
@@ -2696,7 +2705,7 @@
       </c>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>5</v>
       </c>
@@ -2728,7 +2737,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>6</v>
       </c>
@@ -2760,7 +2769,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>6</v>
       </c>
@@ -2790,7 +2799,7 @@
       </c>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>6</v>
       </c>
@@ -2818,7 +2827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>6</v>
       </c>
@@ -2846,7 +2855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>6</v>
       </c>
@@ -2876,7 +2885,7 @@
       </c>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>6</v>
       </c>
@@ -2906,7 +2915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>6</v>
       </c>
@@ -2936,7 +2945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>6</v>
       </c>
@@ -2964,7 +2973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>6</v>
       </c>
@@ -2994,7 +3003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>6</v>
       </c>
@@ -3022,7 +3031,7 @@
       </c>
       <c r="J73" s="3"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>6</v>
       </c>
@@ -3054,7 +3063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>6</v>
       </c>
@@ -3080,7 +3089,7 @@
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>6</v>
       </c>
@@ -3110,7 +3119,7 @@
       </c>
       <c r="J76" s="3"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>7</v>
       </c>
@@ -3140,7 +3149,7 @@
       </c>
       <c r="J77" s="3"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>7</v>
       </c>
@@ -3172,7 +3181,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>7</v>
       </c>
@@ -3202,7 +3211,7 @@
       </c>
       <c r="J79" s="3"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>7</v>
       </c>
@@ -3228,7 +3237,7 @@
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>7</v>
       </c>
@@ -3256,7 +3265,7 @@
       </c>
       <c r="J81" s="3"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>7</v>
       </c>
@@ -3284,7 +3293,7 @@
       </c>
       <c r="J82" s="3"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>7</v>
       </c>
@@ -3312,7 +3321,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>7</v>
       </c>
@@ -3342,7 +3351,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>7</v>
       </c>
@@ -3372,7 +3381,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>7</v>
       </c>
@@ -3402,7 +3411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>7</v>
       </c>
@@ -3430,7 +3439,7 @@
       </c>
       <c r="J87" s="3"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>7</v>
       </c>
@@ -3462,7 +3471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>7</v>
       </c>
@@ -3494,7 +3503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>8</v>
       </c>
@@ -3526,7 +3535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>8</v>
       </c>
@@ -3558,7 +3567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>8</v>
       </c>
@@ -3586,7 +3595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>8</v>
       </c>
@@ -3614,7 +3623,7 @@
       </c>
       <c r="J93" s="3"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>8</v>
       </c>
@@ -3644,7 +3653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>8</v>
       </c>
@@ -3674,7 +3683,7 @@
       </c>
       <c r="J95" s="3"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>8</v>
       </c>
@@ -3704,7 +3713,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>8</v>
       </c>
@@ -3732,7 +3741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>8</v>
       </c>
@@ -3762,7 +3771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>8</v>
       </c>
@@ -3794,7 +3803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>9</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>9</v>
       </c>
@@ -3852,7 +3861,7 @@
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>9</v>
       </c>
@@ -3880,7 +3889,7 @@
       </c>
       <c r="J102" s="3"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>9</v>
       </c>
@@ -3910,7 +3919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>9</v>
       </c>
@@ -3938,7 +3947,7 @@
       </c>
       <c r="J104" s="3"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>9</v>
       </c>
@@ -3966,7 +3975,7 @@
       </c>
       <c r="J105" s="3"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>9</v>
       </c>
@@ -3996,7 +4005,7 @@
       </c>
       <c r="J106" s="3"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>9</v>
       </c>
@@ -4028,7 +4037,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>9</v>
       </c>
@@ -4054,7 +4063,7 @@
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>9</v>
       </c>
@@ -4082,7 +4091,7 @@
       </c>
       <c r="J109" s="3"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>9</v>
       </c>
@@ -4108,7 +4117,7 @@
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>9</v>
       </c>
@@ -4138,7 +4147,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>9</v>
       </c>
@@ -4170,7 +4179,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>10</v>
       </c>
@@ -4198,7 +4207,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>10</v>
       </c>
@@ -4226,7 +4235,7 @@
       </c>
       <c r="J114" s="3"/>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>10</v>
       </c>
@@ -4254,7 +4263,7 @@
       </c>
       <c r="J115" s="3"/>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>10</v>
       </c>
@@ -4284,7 +4293,7 @@
       </c>
       <c r="J116" s="3"/>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>10</v>
       </c>
@@ -4314,7 +4323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>10</v>
       </c>
@@ -4344,7 +4353,7 @@
       </c>
       <c r="J118" s="3"/>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>10</v>
       </c>
@@ -4374,7 +4383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>10</v>
       </c>
@@ -4400,7 +4409,7 @@
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>10</v>
       </c>
@@ -4432,7 +4441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>10</v>
       </c>
@@ -4460,7 +4469,7 @@
       </c>
       <c r="J122" s="3"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>11</v>
       </c>
@@ -4488,7 +4497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
         <v>11</v>
       </c>
@@ -4516,7 +4525,7 @@
       </c>
       <c r="J124" s="3"/>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>11</v>
       </c>
@@ -4544,7 +4553,7 @@
       </c>
       <c r="J125" s="3"/>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>11</v>
       </c>
@@ -4572,7 +4581,7 @@
       </c>
       <c r="J126" s="3"/>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>11</v>
       </c>
@@ -4604,7 +4613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>11</v>
       </c>
@@ -4636,7 +4645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>11</v>
       </c>
@@ -4664,7 +4673,7 @@
       </c>
       <c r="J129" s="3"/>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>11</v>
       </c>
@@ -4696,7 +4705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>11</v>
       </c>
@@ -4726,7 +4735,7 @@
       </c>
       <c r="J131" s="3"/>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>11</v>
       </c>
@@ -4756,7 +4765,7 @@
       </c>
       <c r="J132" s="3"/>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>11</v>
       </c>
@@ -4784,7 +4793,7 @@
       </c>
       <c r="J133" s="3"/>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>11</v>
       </c>
@@ -4816,7 +4825,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>11</v>
       </c>
@@ -4846,7 +4855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>11</v>
       </c>
@@ -4874,7 +4883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>11</v>
       </c>
@@ -4906,7 +4915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>12</v>
       </c>
@@ -4932,7 +4941,7 @@
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>12</v>
       </c>
@@ -4962,7 +4971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>12</v>
       </c>
@@ -4994,7 +5003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>12</v>
       </c>
@@ -5024,7 +5033,7 @@
       </c>
       <c r="J141" s="3"/>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>12</v>
       </c>
@@ -5056,7 +5065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>12</v>
       </c>
@@ -5084,7 +5093,7 @@
       </c>
       <c r="J143" s="3"/>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="3">
         <v>12</v>
       </c>
@@ -5114,7 +5123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>12</v>
       </c>
@@ -5144,7 +5153,7 @@
       </c>
       <c r="J145" s="3"/>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>12</v>
       </c>
@@ -5172,7 +5181,7 @@
       </c>
       <c r="J146" s="3"/>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>12</v>
       </c>
@@ -5204,7 +5213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
         <v>12</v>
       </c>
@@ -5234,7 +5243,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>12</v>
       </c>
@@ -5262,7 +5271,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>12</v>
       </c>
@@ -5294,7 +5303,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>12</v>
       </c>
@@ -5322,7 +5331,7 @@
       </c>
       <c r="J151" s="3"/>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
         <v>12</v>
       </c>
@@ -5354,7 +5363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>13</v>
       </c>
@@ -5382,7 +5391,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>13</v>
       </c>
@@ -5412,7 +5421,7 @@
       </c>
       <c r="J154" s="3"/>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>13</v>
       </c>
@@ -5442,7 +5451,7 @@
       </c>
       <c r="J155" s="3"/>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="3">
         <v>13</v>
       </c>
@@ -5468,7 +5477,7 @@
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>13</v>
       </c>
@@ -5496,7 +5505,7 @@
       </c>
       <c r="J157" s="3"/>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>13</v>
       </c>
@@ -5528,7 +5537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>13</v>
       </c>
@@ -5554,7 +5563,7 @@
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="3">
         <v>13</v>
       </c>
@@ -5586,7 +5595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>13</v>
       </c>
@@ -5618,7 +5627,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>13</v>
       </c>
@@ -5644,7 +5653,7 @@
       <c r="I162" s="3"/>
       <c r="J162" s="3"/>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>14</v>
       </c>
@@ -5670,7 +5679,7 @@
       <c r="I163" s="3"/>
       <c r="J163" s="3"/>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" s="3">
         <v>14</v>
       </c>
@@ -5700,7 +5709,7 @@
       </c>
       <c r="J164" s="3"/>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>14</v>
       </c>
@@ -5728,7 +5737,7 @@
       </c>
       <c r="J165" s="3"/>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="3">
         <v>14</v>
       </c>
@@ -5758,7 +5767,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>14</v>
       </c>
@@ -5786,7 +5795,7 @@
       </c>
       <c r="J167" s="3"/>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" s="3">
         <v>14</v>
       </c>
@@ -5818,7 +5827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
         <v>14</v>
       </c>
@@ -5848,7 +5857,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>14</v>
       </c>
@@ -5876,7 +5885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
         <v>14</v>
       </c>
@@ -5908,7 +5917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" s="3">
         <v>14</v>
       </c>
@@ -5938,7 +5947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" s="3">
         <v>14</v>
       </c>
@@ -5964,7 +5973,7 @@
       <c r="I173" s="3"/>
       <c r="J173" s="3"/>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" s="3">
         <v>15</v>
       </c>
@@ -5990,7 +5999,7 @@
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" s="3">
         <v>15</v>
       </c>
@@ -6018,7 +6027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" s="3">
         <v>15</v>
       </c>
@@ -6048,7 +6057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" s="3">
         <v>15</v>
       </c>
@@ -6078,7 +6087,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" s="3">
         <v>15</v>
       </c>
@@ -6106,7 +6115,7 @@
       </c>
       <c r="J178" s="3"/>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" s="3">
         <v>15</v>
       </c>
@@ -6138,7 +6147,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" s="3">
         <v>15</v>
       </c>
@@ -6168,7 +6177,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" s="3">
         <v>15</v>
       </c>
@@ -6198,7 +6207,7 @@
       </c>
       <c r="J181" s="3"/>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
         <v>15</v>
       </c>
@@ -6228,7 +6237,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" s="3">
         <v>15</v>
       </c>
@@ -6254,7 +6263,7 @@
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" s="3">
         <v>15</v>
       </c>
@@ -6282,7 +6291,7 @@
       </c>
       <c r="J184" s="3"/>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" s="3">
         <v>15</v>
       </c>
@@ -6314,7 +6323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="3">
         <v>15</v>
       </c>
@@ -6344,7 +6353,7 @@
       </c>
       <c r="J186" s="3"/>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="3">
         <v>15</v>
       </c>
@@ -6376,7 +6385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="3">
         <v>15</v>
       </c>
@@ -6404,7 +6413,7 @@
       </c>
       <c r="J188" s="3"/>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" s="3">
         <v>16</v>
       </c>
@@ -6430,7 +6439,7 @@
       <c r="I189" s="3"/>
       <c r="J189" s="3"/>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" s="3">
         <v>16</v>
       </c>
@@ -6458,7 +6467,7 @@
       </c>
       <c r="J190" s="3"/>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="3">
         <v>16</v>
       </c>
@@ -6488,7 +6497,7 @@
       </c>
       <c r="J191" s="3"/>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" s="3">
         <v>16</v>
       </c>
@@ -6516,7 +6525,7 @@
       </c>
       <c r="J192" s="3"/>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" s="3">
         <v>16</v>
       </c>
@@ -6546,7 +6555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" s="3">
         <v>16</v>
       </c>
@@ -6578,7 +6587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" s="3">
         <v>16</v>
       </c>
@@ -6606,7 +6615,7 @@
       <c r="I195" s="3"/>
       <c r="J195" s="3"/>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" s="3">
         <v>16</v>
       </c>
@@ -6636,7 +6645,7 @@
       </c>
       <c r="J196" s="3"/>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" s="3">
         <v>16</v>
       </c>
@@ -6662,7 +6671,7 @@
       <c r="I197" s="3"/>
       <c r="J197" s="3"/>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" s="3">
         <v>16</v>
       </c>
@@ -6690,7 +6699,7 @@
       </c>
       <c r="J198" s="3"/>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>16</v>
       </c>
@@ -6722,7 +6731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" s="3">
         <v>16</v>
       </c>
@@ -6754,7 +6763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>16</v>
       </c>
@@ -6782,7 +6791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" s="3">
         <v>17</v>
       </c>
@@ -6810,7 +6819,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>17</v>
       </c>
@@ -6840,7 +6849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" s="3">
         <v>17</v>
       </c>
@@ -6866,7 +6875,7 @@
       <c r="I204" s="3"/>
       <c r="J204" s="3"/>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>17</v>
       </c>
@@ -6898,7 +6907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" s="3">
         <v>17</v>
       </c>
@@ -6926,7 +6935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
         <v>17</v>
       </c>
@@ -6958,7 +6967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" s="3">
         <v>17</v>
       </c>
@@ -6988,7 +6997,7 @@
       </c>
       <c r="J208" s="3"/>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" s="3">
         <v>17</v>
       </c>
@@ -7016,7 +7025,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" s="3">
         <v>17</v>
       </c>
@@ -7042,7 +7051,7 @@
       <c r="I210" s="3"/>
       <c r="J210" s="3"/>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" s="3">
         <v>17</v>
       </c>
@@ -7074,7 +7083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" s="3">
         <v>17</v>
       </c>
@@ -7102,7 +7111,7 @@
       </c>
       <c r="J212" s="3"/>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" s="3">
         <v>17</v>
       </c>
@@ -7134,7 +7143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" s="3">
         <v>18</v>
       </c>
@@ -7162,7 +7171,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" s="3">
         <v>18</v>
       </c>
@@ -7190,7 +7199,7 @@
       <c r="I215" s="3"/>
       <c r="J215" s="3"/>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" s="3">
         <v>18</v>
       </c>
@@ -7218,7 +7227,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
         <v>18</v>
       </c>
@@ -7248,7 +7257,7 @@
       </c>
       <c r="J217" s="3"/>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" s="3">
         <v>18</v>
       </c>
@@ -7274,7 +7283,7 @@
       <c r="I218" s="3"/>
       <c r="J218" s="3"/>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
         <v>18</v>
       </c>
@@ -7304,7 +7313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" s="3">
         <v>18</v>
       </c>
@@ -7336,7 +7345,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
         <v>18</v>
       </c>
@@ -7362,7 +7371,7 @@
       <c r="I221" s="3"/>
       <c r="J221" s="3"/>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" s="3">
         <v>18</v>
       </c>
@@ -7392,7 +7401,7 @@
       </c>
       <c r="J222" s="3"/>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
         <v>18</v>
       </c>
@@ -7422,7 +7431,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" s="3">
         <v>18</v>
       </c>
@@ -7452,7 +7461,7 @@
       </c>
       <c r="J224" s="3"/>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" s="3">
         <v>18</v>
       </c>
@@ -7482,7 +7491,7 @@
       </c>
       <c r="J225" s="3"/>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" s="3">
         <v>19</v>
       </c>
@@ -7512,7 +7521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227" s="3">
         <v>19</v>
       </c>
@@ -7542,7 +7551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" s="3">
         <v>19</v>
       </c>
@@ -7570,7 +7579,7 @@
       </c>
       <c r="J228" s="3"/>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" s="3">
         <v>19</v>
       </c>
@@ -7602,7 +7611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" s="3">
         <v>19</v>
       </c>
@@ -7630,7 +7639,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" s="3">
         <v>19</v>
       </c>
@@ -7660,7 +7669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" s="3">
         <v>19</v>
       </c>
@@ -7688,7 +7697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" s="3">
         <v>19</v>
       </c>
@@ -7718,7 +7727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" s="3">
         <v>19</v>
       </c>
@@ -7750,7 +7759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" s="3">
         <v>19</v>
       </c>
@@ -7776,7 +7785,7 @@
       <c r="I235" s="3"/>
       <c r="J235" s="3"/>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" s="3">
         <v>19</v>
       </c>
@@ -7806,7 +7815,7 @@
       </c>
       <c r="J236" s="3"/>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" s="3">
         <v>19</v>
       </c>
@@ -7836,7 +7845,7 @@
       </c>
       <c r="J237" s="3"/>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" s="3">
         <v>20</v>
       </c>
@@ -7866,7 +7875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" s="3">
         <v>20</v>
       </c>
@@ -7894,7 +7903,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" s="3">
         <v>20</v>
       </c>
@@ -7922,7 +7931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" s="3">
         <v>20</v>
       </c>
@@ -7950,7 +7959,7 @@
       <c r="I241" s="3"/>
       <c r="J241" s="3"/>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" s="3">
         <v>20</v>
       </c>
@@ -7980,7 +7989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" s="3">
         <v>20</v>
       </c>
@@ -8012,7 +8021,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244" s="3">
         <v>20</v>
       </c>
@@ -8044,7 +8053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245" s="3">
         <v>20</v>
       </c>
@@ -8070,7 +8079,7 @@
       <c r="I245" s="3"/>
       <c r="J245" s="3"/>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" s="3">
         <v>20</v>
       </c>
@@ -8098,7 +8107,7 @@
       </c>
       <c r="J246" s="3"/>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" s="3">
         <v>20</v>
       </c>
@@ -8126,7 +8135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" s="3">
         <v>21</v>
       </c>
@@ -8154,7 +8163,7 @@
       </c>
       <c r="J248" s="3"/>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" s="3">
         <v>21</v>
       </c>
@@ -8184,7 +8193,7 @@
       </c>
       <c r="J249" s="3"/>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" s="3">
         <v>21</v>
       </c>
@@ -8212,7 +8221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" s="3">
         <v>21</v>
       </c>
@@ -8240,7 +8249,7 @@
       <c r="I251" s="3"/>
       <c r="J251" s="3"/>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" s="3">
         <v>21</v>
       </c>
@@ -8272,7 +8281,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" s="3">
         <v>21</v>
       </c>
@@ -8302,7 +8311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" s="3">
         <v>21</v>
       </c>
@@ -8332,7 +8341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" s="3">
         <v>21</v>
       </c>
@@ -8358,7 +8367,7 @@
       <c r="I255" s="3"/>
       <c r="J255" s="3"/>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" s="3">
         <v>21</v>
       </c>
@@ -8386,7 +8395,7 @@
       </c>
       <c r="J256" s="3"/>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" s="3">
         <v>21</v>
       </c>
@@ -8416,7 +8425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" s="3">
         <v>21</v>
       </c>
@@ -8446,7 +8455,7 @@
       </c>
       <c r="J258" s="3"/>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" s="3">
         <v>22</v>
       </c>
@@ -8474,7 +8483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" s="3">
         <v>22</v>
       </c>
@@ -8502,7 +8511,7 @@
       <c r="I260" s="3"/>
       <c r="J260" s="3"/>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" s="3">
         <v>22</v>
       </c>
@@ -8532,7 +8541,7 @@
       </c>
       <c r="J261" s="3"/>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" s="3">
         <v>22</v>
       </c>
@@ -8560,7 +8569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" s="3">
         <v>22</v>
       </c>
@@ -8586,7 +8595,7 @@
       <c r="I263" s="3"/>
       <c r="J263" s="3"/>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" s="3">
         <v>22</v>
       </c>
@@ -8614,7 +8623,7 @@
       </c>
       <c r="J264" s="3"/>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" s="3">
         <v>22</v>
       </c>
@@ -8646,7 +8655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" s="3">
         <v>22</v>
       </c>
@@ -8676,7 +8685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" s="3">
         <v>22</v>
       </c>
@@ -8704,7 +8713,7 @@
       </c>
       <c r="J267" s="3"/>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268" s="3">
         <v>23</v>
       </c>
@@ -8730,7 +8739,7 @@
       <c r="I268" s="3"/>
       <c r="J268" s="3"/>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269" s="3">
         <v>23</v>
       </c>
@@ -8760,7 +8769,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" s="3">
         <v>23</v>
       </c>
@@ -8792,7 +8801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" s="3">
         <v>23</v>
       </c>
@@ -8822,7 +8831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272" s="3">
         <v>23</v>
       </c>
@@ -8850,7 +8859,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" s="3">
         <v>23</v>
       </c>
@@ -8882,7 +8891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" s="3">
         <v>23</v>
       </c>
@@ -8912,7 +8921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275" s="3">
         <v>23</v>
       </c>
@@ -8942,7 +8951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" s="3">
         <v>24</v>
       </c>
@@ -8970,7 +8979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" s="3">
         <v>24</v>
       </c>
@@ -9000,7 +9009,7 @@
       </c>
       <c r="J277" s="3"/>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" s="3">
         <v>24</v>
       </c>
@@ -9030,7 +9039,7 @@
       </c>
       <c r="J278" s="3"/>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279" s="3">
         <v>24</v>
       </c>
@@ -9060,7 +9069,7 @@
       </c>
       <c r="J279" s="3"/>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" s="3">
         <v>24</v>
       </c>
@@ -9090,7 +9099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" s="3">
         <v>24</v>
       </c>
@@ -9120,7 +9129,7 @@
       </c>
       <c r="J281" s="3"/>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282" s="3">
         <v>24</v>
       </c>
@@ -9152,7 +9161,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283" s="3">
         <v>24</v>
       </c>
@@ -9180,7 +9189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284" s="3">
         <v>24</v>
       </c>
@@ -9208,7 +9217,7 @@
       </c>
       <c r="J284" s="3"/>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" s="3">
         <v>24</v>
       </c>
@@ -9236,7 +9245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" s="3">
         <v>24</v>
       </c>
@@ -9266,7 +9275,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A287" s="3">
         <v>24</v>
       </c>
@@ -9296,7 +9305,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288" s="3">
         <v>24</v>
       </c>
@@ -9325,13 +9334,13 @@
       <c r="J288" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J288" xr:uid="{05A13303-F17E-43F6-BB44-847982700F32}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J288">
+  <autoFilter ref="A1:J288">
+    <sortState ref="A2:J288">
       <sortCondition ref="B2:B288"/>
       <sortCondition ref="C2:C288"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J288">
+  <sortState ref="A2:J288">
     <sortCondition ref="A1:A288"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9349,6 +9358,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF8BA7DE477F3446865215AD96F68BC1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="712890d8b247e388906a591dbe84e72e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c59d9f10-5f45-47e1-9538-4f341ec0dbef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20bdc581e2bd72745e5c359b924c6aa9" ns2:_="">
     <xsd:import namespace="c59d9f10-5f45-47e1-9538-4f341ec0dbef"/>
@@ -9480,20 +9495,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C22C9E5-3D50-452A-ADA9-D2EA797D2772}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C22C9E5-3D50-452A-ADA9-D2EA797D2772}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EAAF513-65B9-41AF-A266-BB1EB37D27A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4FCD2FC-53D6-433C-831B-DBCB9E4F5CCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4FCD2FC-53D6-433C-831B-DBCB9E4F5CCB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EAAF513-65B9-41AF-A266-BB1EB37D27A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c59d9f10-5f45-47e1-9538-4f341ec0dbef"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>